<commit_message>
se corrige para que no se pueda borrar articulo si no es de sucursal y se inicia el informe de errores de importacion
</commit_message>
<xml_diff>
--- a/ejemploinventarios.xlsx
+++ b/ejemploinventarios.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
         <v>17</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K2">
         <v>1</v>

</xml_diff>

<commit_message>
se corrige importacion de registros en productos, se incluyen mensajes de error al eliminar sucursales y categorias y no se puede ni actualizar sucursal y categoria general
</commit_message>
<xml_diff>
--- a/ejemploinventarios.xlsx
+++ b/ejemploinventarios.xlsx
@@ -396,15 +396,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -480,7 +482,7 @@
         <v>17</v>
       </c>
       <c r="J2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>1</v>

</xml_diff>